<commit_message>
Lab 3: Fixed test count
</commit_message>
<xml_diff>
--- a/Lab3-QuickSort/Lab3Graph.xlsx
+++ b/Lab3-QuickSort/Lab3Graph.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Size (10000 tests)</t>
+    <t>Size (100000 tests)</t>
   </si>
   <si>
     <t>Insert, ms</t>
@@ -199,11 +199,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="645323346"/>
-        <c:axId val="521452663"/>
+        <c:axId val="260365406"/>
+        <c:axId val="199167070"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="645323346"/>
+        <c:axId val="260365406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -255,10 +255,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="521452663"/>
+        <c:crossAx val="199167070"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="521452663"/>
+        <c:axId val="199167070"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,7 +333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="645323346"/>
+        <c:crossAx val="260365406"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>